<commit_message>
feat: updated data, remove unneeded columns
</commit_message>
<xml_diff>
--- a/src/python/excel/Job Search Tracker.xlsx
+++ b/src/python/excel/Job Search Tracker.xlsx
@@ -60,12 +60,12 @@
         <t xml:space="preserve">This sheet should include people you have reached out to, spoke with as well as people you are planning to reach out to in order to keep track of them</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F1">
+    <comment authorId="0" ref="G1">
       <text>
         <t xml:space="preserve">What is the reason for connecting around your current job search. I.e. - do they work at Amazon and you want to learn more about working there? Are they an expect in AI and you'd like to discuss your career with them? Did a friend said they'd be a good connection for you?</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G1">
+    <comment authorId="0" ref="H1">
       <text>
         <t xml:space="preserve">Did you already connect with them? Are you in active conversation with them?</t>
       </text>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -86,15 +86,21 @@
     <t>Keyword</t>
   </si>
   <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
+  </si>
+  <si>
     <t>Company</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>KeywordID</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -104,6 +110,15 @@
     <t>Job Posting URL</t>
   </si>
   <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Hard Skill</t>
+  </si>
+  <si>
+    <t>Soft Skill</t>
+  </si>
+  <si>
     <t>Job Description</t>
   </si>
   <si>
@@ -125,42 +140,57 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>CompanyID</t>
-  </si>
-  <si>
-    <t>Support</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Linux</t>
-  </si>
-  <si>
-    <t>Hard Skill</t>
-  </si>
-  <si>
-    <t>Customer Service</t>
-  </si>
-  <si>
-    <t>Soft Skill</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
-    <t>Portland</t>
+    <t>Portland, OR</t>
   </si>
   <si>
     <t>CSA</t>
   </si>
   <si>
+    <t>Waiting for TN</t>
+  </si>
+  <si>
+    <t>Follow-up on TN form</t>
+  </si>
+  <si>
+    <t>Quantum World</t>
+  </si>
+  <si>
+    <t>Halifax, NS</t>
+  </si>
+  <si>
+    <t>Sr. Java Developer</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1WdM9Tkg2_AFNaA78bNxmA_IAVBSNg6q-Fvr0WfkZ8Z4/edit</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1k8agLFAs4WGqdR9PGbdUDs8EZlLRoE8WeLDuQhH3m8U/edit#heading=h.69u6162ojm4</t>
+  </si>
+  <si>
+    <t>Sent Resume</t>
+  </si>
+  <si>
+    <t>TMC</t>
+  </si>
+  <si>
+    <t>Montreal, QC</t>
+  </si>
+  <si>
+    <t>Full Stack Developer</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
     <t>LinkedIn Profile</t>
   </si>
   <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>Connection Description</t>
   </si>
   <si>
@@ -171,13 +201,55 @@
   </si>
   <si>
     <t>Manager</t>
+  </si>
+  <si>
+    <t>Rohit Gaur</t>
+  </si>
+  <si>
+    <t>Recruiter</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rohit-kumar-gaur-34113916b/</t>
+  </si>
+  <si>
+    <t>rohitgaur@quantumworld.us</t>
+  </si>
+  <si>
+    <t>Contacted by Email</t>
+  </si>
+  <si>
+    <t>Soukaina Chakri</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/soukaina-chakri-4610a584/</t>
+  </si>
+  <si>
+    <t>soukaina.chakri@tmc-employeneurs.com</t>
+  </si>
+  <si>
+    <t>Contacted by LinkedIn</t>
+  </si>
+  <si>
+    <t>Tiona Corcoran</t>
+  </si>
+  <si>
+    <t>Global Talent Accelerator</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/tionacorcoran/</t>
+  </si>
+  <si>
+    <t>LinkedIn message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -187,6 +259,14 @@
       <b/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -212,7 +292,16 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -256,75 +345,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" s="3">
+        <v>43807.0</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3">
+        <v>43936.0</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="3">
+        <v>43936.0</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="F3"/>
+    <hyperlink r:id="rId3" location="heading=h.69u6162ojm4" ref="H3"/>
+    <hyperlink r:id="rId4" location="heading=h.69u6162ojm4" ref="H4"/>
+  </hyperlinks>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -346,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
@@ -354,10 +487,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -365,10 +498,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -376,10 +509,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -407,9 +540,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2">
@@ -419,38 +550,29 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" s="2">
         <v>1.0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" s="2">
         <v>1.0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3.0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -469,7 +591,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="5" max="5" width="15.14"/>
-    <col customWidth="1" min="6" max="6" width="22.14"/>
+    <col customWidth="1" min="6" max="7" width="22.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -477,68 +599,147 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="2">
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="2">
-        <v>1.0</v>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="E3"/>
+    <hyperlink r:id="rId3" ref="E4"/>
+    <hyperlink r:id="rId4" ref="F4"/>
+    <hyperlink r:id="rId5" ref="E5"/>
+  </hyperlinks>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>